<commit_message>
Correction in agriculture data
</commit_message>
<xml_diff>
--- a/prep/CW/cw_nutrient_trend_mse2019.xlsx
+++ b/prep/CW/cw_nutrient_trend_mse2019.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Hurtadoyhurtado\carpeta compartida\PROYECTOS\CI IdSO MANABÍ Y SANTA ELENA\CAPAS DE DATOS\DATOS CRUDOS\05 AGUAS LIMPIAS\AGUAS LIMPIAS 2019\DATOS CRUDOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Hurtadoyhurtado\carpeta compartida\PROYECTOS\CI IdSO MANABÍ Y SANTA ELENA\CAPAS DE DATOS\05 AGUAS LIMPIAS\AGUAS LIMPIAS 2019\DATOS CRUDOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19755" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19755" windowHeight="11760" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cw_nutrients_trendgl" sheetId="1" r:id="rId1"/>
@@ -467,6 +467,1553 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-EC" b="1"/>
+              <a:t>USO</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-EC" b="1" baseline="0"/>
+              <a:t> DE FERTILIZANTES - ECUADOR</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-EC" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.23468044619422573"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>cw_nutrients_trendgl!$A$3:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cw_nutrients_trendgl!$B$3:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>50.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70.44</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68.33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60.63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>81.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>69.78</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>81.34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="272798240"/>
+        <c:axId val="272807200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="272798240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Año</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-EC"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="272807200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="2"/>
+        <c:tickMarkSkip val="2"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="272807200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-EC"/>
+                  <a:t>Uso (kg/ha)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-EC"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="272798240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-EC"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TENDENCIA SANTA ELENA 2016</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15425787401574803"/>
+                  <c:y val="-0.32036490230387871"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-EC"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'cw_nutrients_trend MSE'!$A$5:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'cw_nutrients_trend MSE'!$F$5:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>476.46508999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>487.40457000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>815.54160000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>337.87476000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>535.54256000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-989C-4132-BB13-255599590109}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="455232512"/>
+        <c:axId val="455233072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="455232512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455233072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="455233072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455232512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-EC"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tendencia de contaminación por nutrientes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Manabí</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[3]cw_chemical_trend!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cw_nutrients_trend!$C$6:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-2.5290183752011343E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14955745839056434</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13854118873448723</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48568908211230566</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99B6-4CA8-A17A-94F5AA14B184}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Santa Elena</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[3]cw_chemical_trend!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cw_nutrients_trend!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.41583533401106598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.86305377778174219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.23675840618693336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.292476265155124E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-99B6-4CA8-A17A-94F5AA14B184}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="455226912"/>
+        <c:axId val="455227472"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="455226912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Año</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-EC"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455227472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="455227472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tendencia</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-EC"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="455226912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-EC"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-EC"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -486,6 +2033,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -652,7 +2200,7 @@
                   <c:v>311901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>713580</c:v>
+                  <c:v>351681</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>347672</c:v>
@@ -783,12 +2331,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="35529856"/>
-        <c:axId val="35530416"/>
+        <c:axId val="272810560"/>
+        <c:axId val="272808880"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="35529856"/>
+        <c:axId val="272810560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,7 +2373,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35530416"/>
+        <c:crossAx val="272808880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -833,7 +2381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35530416"/>
+        <c:axId val="272808880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +2432,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35529856"/>
+        <c:crossAx val="272810560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -972,583 +2520,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>TENDENCIA DE CONTAMINACIÓN POR</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> NUTRIENTES</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>SANTA ELENA</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>[3]cw_chemical_trend!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2016</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>cw_nutrients_trend!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.41583533401106598</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.86305377778174219</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.23675840618693336</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-3.292476265155124E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-99B6-4CA8-A17A-94F5AA14B184}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>MANABÍ</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>[3]cw_chemical_trend!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2016</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>cw_nutrients_trend!$C$6:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>-2.5290183752011343E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.14955745839056434</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="1"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-99B6-4CA8-A17A-94F5AA14B184}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="562642416"/>
-        <c:axId val="229749648"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="562642416"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Año</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-EC"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="229749648"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickMarkSkip val="1"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="229749648"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tendencia</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-EC"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="562642416"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
-          </a:p>
-        </c:txPr>
-      </c:dTable>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-EC"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -1588,6 +2560,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1676,6 +2649,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.13799037620297464"/>
+                  <c:y val="-0.18684406033533077"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1769,11 +2748,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="289363840"/>
-        <c:axId val="289364400"/>
+        <c:axId val="272803280"/>
+        <c:axId val="272803840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="289363840"/>
+        <c:axId val="272803280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,12 +2809,12 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289364400"/>
+        <c:crossAx val="272803840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="289364400"/>
+        <c:axId val="272803840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1892,7 +2871,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289363840"/>
+        <c:crossAx val="272803280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1948,7 +2927,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -1988,6 +2967,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2076,6 +3056,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2169,11 +3150,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="35292832"/>
-        <c:axId val="35293392"/>
+        <c:axId val="455248192"/>
+        <c:axId val="455248752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="35292832"/>
+        <c:axId val="455248192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2230,12 +3211,12 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35293392"/>
+        <c:crossAx val="455248752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35293392"/>
+        <c:axId val="455248752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2292,7 +3273,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35292832"/>
+        <c:crossAx val="455248192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2348,7 +3329,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -2388,6 +3369,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2575,11 +3557,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227834848"/>
-        <c:axId val="227835408"/>
+        <c:axId val="455247072"/>
+        <c:axId val="455243712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227834848"/>
+        <c:axId val="455247072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,12 +3618,12 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227835408"/>
+        <c:crossAx val="455243712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="227835408"/>
+        <c:axId val="455243712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,7 +3680,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227834848"/>
+        <c:crossAx val="455247072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2754,7 +3736,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -2794,6 +3776,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2882,6 +3865,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2975,11 +3959,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227837648"/>
-        <c:axId val="227838208"/>
+        <c:axId val="455242592"/>
+        <c:axId val="455243152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227837648"/>
+        <c:axId val="455242592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3036,12 +4020,12 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227838208"/>
+        <c:crossAx val="455243152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="227838208"/>
+        <c:axId val="455243152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3098,7 +4082,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227837648"/>
+        <c:crossAx val="455242592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3154,7 +4138,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -3194,6 +4178,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3361,7 +4346,7 @@
                   <c:v>25295.1711</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49793.612399999998</c:v>
+                  <c:v>24540.300179999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3381,11 +4366,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="395629328"/>
-        <c:axId val="395629888"/>
+        <c:axId val="455241472"/>
+        <c:axId val="455239792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="395629328"/>
+        <c:axId val="455241472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3442,12 +4427,12 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395629888"/>
+        <c:crossAx val="455239792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="395629888"/>
+        <c:axId val="455239792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3504,7 +4489,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395629328"/>
+        <c:crossAx val="455241472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3560,7 +4545,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -3600,6 +4585,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3787,11 +4773,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="395632128"/>
-        <c:axId val="395632688"/>
+        <c:axId val="455235872"/>
+        <c:axId val="455236432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="395632128"/>
+        <c:axId val="455235872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3848,12 +4834,12 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395632688"/>
+        <c:crossAx val="455236432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="395632688"/>
+        <c:axId val="455236432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3910,7 +4896,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395632128"/>
+        <c:crossAx val="455235872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3966,7 +4952,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -4006,6 +4992,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4170,7 +5157,7 @@
                   <c:v>25295.1711</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49793.612399999998</c:v>
+                  <c:v>24540.300179999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>28279.640480000002</c:v>
@@ -4193,11 +5180,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="395634928"/>
-        <c:axId val="225906304"/>
+        <c:axId val="455234192"/>
+        <c:axId val="455234752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="395634928"/>
+        <c:axId val="455234192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4254,12 +5241,12 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225906304"/>
+        <c:crossAx val="455234752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="225906304"/>
+        <c:axId val="455234752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4316,413 +5303,7 @@
             <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395634928"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-EC"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>TENDENCIA SANTA ELENA 2016</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.15425787401574803"/>
-                  <c:y val="-0.32036490230387871"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="es-EC"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'cw_nutrients_trend MSE'!$A$5:$A$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2016</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'cw_nutrients_trend MSE'!$F$5:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>476.46508999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>487.40457000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>815.54160000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>337.87476000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>535.54256000000009</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-989C-4132-BB13-255599590109}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="225908544"/>
-        <c:axId val="225909104"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="225908544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="225909104"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="225909104"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="225908544"/>
+        <c:crossAx val="455234192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4819,6 +5400,46 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5179,7 +5800,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5202,6 +5823,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -5297,7 +5929,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -5329,10 +5961,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5653,6 +6285,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6188,7 +6831,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6704,8 +7347,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6728,17 +7371,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -6834,7 +7466,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -6866,10 +7498,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -7190,17 +7822,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -7220,7 +7841,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7736,7 +8357,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8252,7 +8873,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8768,7 +9389,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9284,7 +9905,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9800,7 +10421,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10316,7 +10937,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10353,7 +11525,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10646,20 +11818,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11195,8 +12367,8 @@
       <sheetName val="GR 57"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="13">
           <cell r="C13">
@@ -11209,9 +12381,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
       <sheetData sheetId="6">
         <row r="19">
           <cell r="C19">
@@ -11234,99 +12406,99 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-      <sheetData sheetId="61" refreshError="1"/>
-      <sheetData sheetId="62" refreshError="1"/>
-      <sheetData sheetId="63" refreshError="1"/>
-      <sheetData sheetId="64" refreshError="1"/>
-      <sheetData sheetId="65" refreshError="1"/>
-      <sheetData sheetId="66" refreshError="1"/>
-      <sheetData sheetId="67" refreshError="1"/>
-      <sheetData sheetId="68" refreshError="1"/>
-      <sheetData sheetId="69" refreshError="1"/>
-      <sheetData sheetId="70" refreshError="1"/>
-      <sheetData sheetId="71" refreshError="1"/>
-      <sheetData sheetId="72" refreshError="1"/>
-      <sheetData sheetId="73" refreshError="1"/>
-      <sheetData sheetId="74" refreshError="1"/>
-      <sheetData sheetId="75" refreshError="1"/>
-      <sheetData sheetId="76" refreshError="1"/>
-      <sheetData sheetId="77" refreshError="1"/>
-      <sheetData sheetId="78" refreshError="1"/>
-      <sheetData sheetId="79" refreshError="1"/>
-      <sheetData sheetId="80" refreshError="1"/>
-      <sheetData sheetId="81" refreshError="1"/>
-      <sheetData sheetId="82" refreshError="1"/>
-      <sheetData sheetId="83" refreshError="1"/>
-      <sheetData sheetId="84" refreshError="1"/>
-      <sheetData sheetId="85" refreshError="1"/>
-      <sheetData sheetId="86" refreshError="1"/>
-      <sheetData sheetId="87" refreshError="1"/>
-      <sheetData sheetId="88" refreshError="1"/>
-      <sheetData sheetId="89" refreshError="1"/>
-      <sheetData sheetId="90" refreshError="1"/>
-      <sheetData sheetId="91" refreshError="1"/>
-      <sheetData sheetId="92" refreshError="1"/>
-      <sheetData sheetId="93" refreshError="1"/>
-      <sheetData sheetId="94" refreshError="1"/>
-      <sheetData sheetId="95" refreshError="1"/>
-      <sheetData sheetId="96" refreshError="1"/>
-      <sheetData sheetId="97" refreshError="1"/>
-      <sheetData sheetId="98" refreshError="1"/>
-      <sheetData sheetId="99" refreshError="1"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79"/>
+      <sheetData sheetId="80"/>
+      <sheetData sheetId="81"/>
+      <sheetData sheetId="82"/>
+      <sheetData sheetId="83"/>
+      <sheetData sheetId="84"/>
+      <sheetData sheetId="85"/>
+      <sheetData sheetId="86"/>
+      <sheetData sheetId="87"/>
+      <sheetData sheetId="88"/>
+      <sheetData sheetId="89"/>
+      <sheetData sheetId="90"/>
+      <sheetData sheetId="91"/>
+      <sheetData sheetId="92"/>
+      <sheetData sheetId="93"/>
+      <sheetData sheetId="94"/>
+      <sheetData sheetId="95"/>
+      <sheetData sheetId="96"/>
+      <sheetData sheetId="97"/>
+      <sheetData sheetId="98"/>
+      <sheetData sheetId="99"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -11350,52 +12522,20 @@
           <cell r="B2">
             <v>2013</v>
           </cell>
-          <cell r="C2">
-            <v>-1</v>
-          </cell>
         </row>
         <row r="3">
           <cell r="B3">
             <v>2014</v>
-          </cell>
-          <cell r="C3">
-            <v>-0.71752132933687496</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
             <v>2015</v>
           </cell>
-          <cell r="C4">
-            <v>-9.6371198857713777E-3</v>
-          </cell>
         </row>
         <row r="5">
           <cell r="B5">
             <v>2016</v>
-          </cell>
-          <cell r="C5">
-            <v>-1.9896991517898269E-2</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>-1</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>-0.84528505522019615</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9">
-            <v>1</v>
           </cell>
         </row>
       </sheetData>
@@ -11667,7 +12807,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B17"/>
@@ -11859,9 +12999,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <f>AVERAGE(B3:B17)</f>
+        <v>60.998000000000005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11869,8 +13016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U116"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65:K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12347,7 +13494,7 @@
         <v>47373</v>
       </c>
       <c r="H13" s="26">
-        <v>414518</v>
+        <v>52619</v>
       </c>
       <c r="I13" s="30">
         <v>41112</v>
@@ -12361,7 +13508,7 @@
       </c>
       <c r="L13" s="28">
         <f t="shared" si="0"/>
-        <v>88394.022043372912</v>
+        <v>48183.022043372926</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -13072,7 +14219,7 @@
       </c>
       <c r="H32" s="17">
         <f t="shared" si="1"/>
-        <v>713580</v>
+        <v>351681</v>
       </c>
       <c r="I32" s="17">
         <f t="shared" si="1"/>
@@ -13088,7 +14235,7 @@
       </c>
       <c r="L32" s="28">
         <f t="shared" si="0"/>
-        <v>367092.10425938643</v>
+        <v>326881.10425938643</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -15899,7 +17046,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15994,7 +17141,7 @@
         <v>20044.804399999997</v>
       </c>
       <c r="F3" s="16">
-        <f t="shared" ref="F3:F9" si="1">D3*C3/1000</f>
+        <f>D3*C3/1000</f>
         <v>390.13211999999999</v>
       </c>
       <c r="G3" s="3"/>
@@ -16027,7 +17174,7 @@
         <v>23481.10356</v>
       </c>
       <c r="F4" s="16">
-        <f t="shared" si="1"/>
+        <f>D4*C4/1000</f>
         <v>664.81272000000001</v>
       </c>
       <c r="G4" s="3"/>
@@ -16060,7 +17207,7 @@
         <v>20907.40841</v>
       </c>
       <c r="F5" s="16">
-        <f t="shared" si="1"/>
+        <f>D5*C5/1000</f>
         <v>476.46508999999998</v>
       </c>
       <c r="G5" s="3"/>
@@ -16093,7 +17240,7 @@
         <v>18976.03803</v>
       </c>
       <c r="F6" s="16">
-        <f t="shared" si="1"/>
+        <f>D6*C6/1000</f>
         <v>487.40457000000004</v>
       </c>
       <c r="G6" s="3">
@@ -16103,11 +17250,11 @@
         <v>31.166</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" ref="I6:J9" si="2">(G6/E2)*5</f>
+        <f>(G6/E2)*5</f>
         <v>-2.5290183752011343E-2</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="2"/>
+        <f>(H6/F2)*5</f>
         <v>0.41583533401106598</v>
       </c>
       <c r="M6" s="8"/>
@@ -16136,7 +17283,7 @@
         <v>25295.1711</v>
       </c>
       <c r="F7" s="16">
-        <f t="shared" si="1"/>
+        <f>D7*C7/1000</f>
         <v>815.54160000000002</v>
       </c>
       <c r="G7" s="3">
@@ -16146,11 +17293,11 @@
         <v>67.340999999999994</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="2"/>
+        <f>(G7/E3)*5</f>
         <v>0.14955745839056434</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="2"/>
+        <f>(H7/F3)*5</f>
         <v>0.86305377778174219</v>
       </c>
       <c r="M7" s="8"/>
@@ -16165,7 +17312,7 @@
       </c>
       <c r="B8" s="15">
         <f>'HECTAREAS PLANTADAS MSE'!H32</f>
-        <v>713580</v>
+        <v>351681</v>
       </c>
       <c r="C8" s="14">
         <f>'HECTAREAS PLANTADAS MSE'!H65</f>
@@ -16175,25 +17322,25 @@
         <v>69.78</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" si="0"/>
-        <v>49793.612399999998</v>
+        <f>D8*B8/1000</f>
+        <v>24540.300179999998</v>
       </c>
       <c r="F8" s="16">
-        <f t="shared" si="1"/>
+        <f>D8*C8/1000</f>
         <v>337.87476000000004</v>
       </c>
       <c r="G8" s="3">
-        <v>5701.3</v>
+        <v>650.62</v>
       </c>
       <c r="H8" s="3">
         <v>-31.48</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="2"/>
-        <v>1.2140187503180537</v>
+        <f>(G8/E4)*5</f>
+        <v>0.13854118873448723</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" si="2"/>
+        <f>(H8/F4)*5</f>
         <v>-0.23675840618693336</v>
       </c>
       <c r="M8" s="8"/>
@@ -16222,21 +17369,21 @@
         <v>28279.640480000002</v>
       </c>
       <c r="F9" s="16">
-        <f t="shared" si="1"/>
+        <f>D9*C9/1000</f>
         <v>535.54256000000009</v>
       </c>
       <c r="G9" s="3">
-        <v>4556.2</v>
+        <v>2030.9</v>
       </c>
       <c r="H9" s="3">
         <v>-3.1375000000000002</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="2"/>
-        <v>1.0896137652863691</v>
+        <f>(G9/E5)*5</f>
+        <v>0.48568908211230566</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="2"/>
+        <f>(H9/F5)*5</f>
         <v>-3.292476265155124E-2</v>
       </c>
       <c r="M9" s="8"/>
@@ -16255,8 +17402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16355,7 +17502,8 @@
         <v>2015</v>
       </c>
       <c r="C8" s="4">
-        <v>1</v>
+        <f>'cw_nutrients_trend MSE'!I8</f>
+        <v>0.13854118873448723</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -16366,7 +17514,8 @@
         <v>2016</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
+        <f>'cw_nutrients_trend MSE'!I9</f>
+        <v>0.48568908211230566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>